<commit_message>
- Function `createScenarios` gets a new argument `stopIfParameterNotFound`. If `TRUE` (default), a scenario will not be created and an error is thrown if any user-defined parameter (e.g., provided in Excel files) is not found in the simulation. If `FALSE`, non-existing parameters are ignored.
- Constructor of a `Scenario` class gets a new argument `stopIfParameterNotFound`.
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/ModelParameters.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/ModelParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esqlabs.sharepoint.com/sites/Services/Freigegebene Dokumente/_Project_template_V02.00/WP1_V00.01/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1550" documentId="13_ncr:1_{4B2F205E-FEDC-4EE6-8C1F-DD0552DF0F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C3F8D02-8689-4DA2-88B4-3EB0BC12FE16}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B167FCB5-A723-4CEB-B5FA-F66EE529A342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22282" yWindow="727" windowWidth="24038" windowHeight="13133" tabRatio="976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Container Path</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>Organism|Liver</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>bar</t>
   </si>
 </sst>
 </file>
@@ -106,9 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -391,54 +395,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -455,33 +460,33 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>-0.1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -491,6 +496,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -727,27 +752,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDADFA4D-689E-4192-9812-F7D7F3DFE5E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -764,23 +788,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Create a separate scenario with definition of missing parameter for testing
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/ModelParameters.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/ModelParameters.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B167FCB5-A723-4CEB-B5FA-F66EE529A342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB0FD69-DC95-4725-8A79-C5A6F5C1746C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="5" r:id="rId1"/>
-    <sheet name="Aciclovir" sheetId="6" r:id="rId2"/>
+    <sheet name="MissingParam" sheetId="7" r:id="rId2"/>
+    <sheet name="Aciclovir" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Container Path</t>
   </si>
@@ -397,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -453,6 +454,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB1D1D3-9309-4BAC-A19A-8F08944F068E}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003F998E-5869-417D-A696-38B00449383B}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -496,26 +537,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -752,26 +773,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDADFA4D-689E-4192-9812-F7D7F3DFE5E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -788,4 +810,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
#559 Add `stopIfParameterNotFound` argument to `createScenarios` function. (#615)
* - Function `createScenarios` gets a new argument `stopIfParameterNotFound`.
If `TRUE` (default), a scenario will not be created and an error is thrown if
any user-defined parameter (e.g., provided in Excel files) is not found in the
simulation. If `FALSE`, non-existing parameters are ignored.

- Constructor of a `Scenario` class gets a new argument `stopIfParameterNotFound`.

* - Update docs
- Styler

* - Create a separate scenario with definition of missing parameter for testing

* Update excel file for tests
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Parameters/ModelParameters.xlsx
+++ b/inst/extdata/examples/TestProject/Parameters/ModelParameters.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esqlabs.sharepoint.com/sites/Services/Freigegebene Dokumente/_Project_template_V02.00/WP1_V00.01/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1550" documentId="13_ncr:1_{4B2F205E-FEDC-4EE6-8C1F-DD0552DF0F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C3F8D02-8689-4DA2-88B4-3EB0BC12FE16}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7725A3FF-868A-49D2-A5A6-8E1FEFEB530E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22282" yWindow="727" windowWidth="24038" windowHeight="13133" tabRatio="976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="5" r:id="rId1"/>
-    <sheet name="Aciclovir" sheetId="6" r:id="rId2"/>
+    <sheet name="MissingParam" sheetId="7" r:id="rId2"/>
+    <sheet name="Aciclovir" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Container Path</t>
   </si>
@@ -62,6 +63,12 @@
   </si>
   <si>
     <t>Organism|Liver</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>bar</t>
   </si>
 </sst>
 </file>
@@ -106,9 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -391,54 +396,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -448,6 +443,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB1D1D3-9309-4BAC-A19A-8F08944F068E}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003F998E-5869-417D-A696-38B00449383B}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -455,33 +490,33 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>-0.1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -491,6 +526,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -727,27 +782,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDADFA4D-689E-4192-9812-F7D7F3DFE5E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -764,23 +818,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>